<commit_message>
all components changed courier frontend download
</commit_message>
<xml_diff>
--- a/server/files/orders.xlsx
+++ b/server/files/orders.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>No</t>
   </si>
@@ -40,70 +40,55 @@
     <t>O'zgartirilgan sana</t>
   </si>
   <si>
-    <t>Mashrab</t>
-  </si>
-  <si>
-    <t>+998946775454</t>
-  </si>
-  <si>
-    <t>STORE_OWNER: sinadigan narsa bor</t>
+    <t>dgfsdgdf</t>
+  </si>
+  <si>
+    <t>+998908171355</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: sdfgdsfg</t>
   </si>
   <si>
     <t>DELIVERED</t>
   </si>
   <si>
-    <t>Bobur</t>
-  </si>
-  <si>
-    <t>STORE_OWNER: arzonroq narsa COURIER: kutilmoqad</t>
+    <t>fdsgsdfg</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: fdsdfsdf</t>
+  </si>
+  <si>
+    <t>sdfgsdf</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: bjkbbbhjs</t>
+  </si>
+  <si>
+    <t>dfgdsg</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: bnjhbhjb COURIER: sdfsdfds</t>
+  </si>
+  <si>
+    <t>REJECTED_DELIVERING</t>
+  </si>
+  <si>
+    <t>bfdfbs</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: nhbdfbhvbf COURIER: dgdfg</t>
   </si>
   <si>
     <t>PENDING</t>
   </si>
   <si>
-    <t>Baxrom</t>
-  </si>
-  <si>
-    <t>+998936979876</t>
-  </si>
-  <si>
-    <t>STORE_OWNER: Tezroq olib kellarin COURIER: SOTILDI</t>
+    <t>sdgdfsgq</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: fdsfsdf COURIER: sfsafs</t>
   </si>
   <si>
     <t>SOLD</t>
-  </si>
-  <si>
-    <t>Suxrob</t>
-  </si>
-  <si>
-    <t>+998945677655</t>
-  </si>
-  <si>
-    <t>STORE_OWNER: rergrg COURIER: dsgdrfd</t>
-  </si>
-  <si>
-    <t>Abdumalik</t>
-  </si>
-  <si>
-    <t>+998946777865</t>
-  </si>
-  <si>
-    <t>STORE_OWNER: tez kelsin COURIER: qat=yt</t>
-  </si>
-  <si>
-    <t>REJECTED</t>
-  </si>
-  <si>
-    <t>STORE_OWNER: Tezroq olib kellarin</t>
-  </si>
-  <si>
-    <t>Bunyod</t>
-  </si>
-  <si>
-    <t>+998936979875</t>
-  </si>
-  <si>
-    <t>NEW</t>
   </si>
 </sst>
 </file>
@@ -492,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -550,13 +535,13 @@
         <v>50000</v>
       </c>
       <c r="G2" s="2">
-        <v>1486562</v>
+        <v>12222</v>
       </c>
       <c r="H2" s="3">
-        <v>44880.49430554398</v>
+        <v>44881.44031289352</v>
       </c>
       <c r="I2" s="3">
-        <v>44880.49517023149</v>
+        <v>44881.443963356476</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -573,19 +558,19 @@
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2">
         <v>50000</v>
       </c>
       <c r="G3" s="2">
-        <v>1430319</v>
+        <v>10000</v>
       </c>
       <c r="H3" s="3">
-        <v>44880.49430554398</v>
+        <v>44881.449103900464</v>
       </c>
       <c r="I3" s="3">
-        <v>44880.50429887732</v>
+        <v>44881.450163761576</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -593,28 +578,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2">
         <v>50000</v>
       </c>
       <c r="G4" s="2">
-        <v>111704296</v>
+        <v>122219</v>
       </c>
       <c r="H4" s="3">
-        <v>44880.49430550926</v>
+        <v>44881.449103900464</v>
       </c>
       <c r="I4" s="3">
-        <v>44880.50671046296</v>
+        <v>44881.450163761576</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -622,13 +607,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
@@ -637,13 +622,13 @@
         <v>50000</v>
       </c>
       <c r="G5" s="2">
-        <v>10624</v>
+        <v>1222</v>
       </c>
       <c r="H5" s="3">
-        <v>44880.494305520835</v>
+        <v>44881.44031289352</v>
       </c>
       <c r="I5" s="3">
-        <v>44880.51017487269</v>
+        <v>44881.4628338426</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -651,28 +636,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2">
         <v>50000</v>
       </c>
       <c r="G6" s="2">
-        <v>1150296</v>
+        <v>12222</v>
       </c>
       <c r="H6" s="3">
-        <v>44880.494305520835</v>
+        <v>44881.44031289352</v>
       </c>
       <c r="I6" s="3">
-        <v>44880.51154866898</v>
+        <v>44881.46646645833</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -683,51 +668,25 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2">
         <v>50000</v>
       </c>
       <c r="G7" s="2">
-        <v>76590000</v>
+        <v>111111</v>
       </c>
       <c r="H7" s="3">
-        <v>44881.223896446754</v>
+        <v>44881.44031289352</v>
       </c>
       <c r="I7" s="3">
-        <v>44881.22546621528</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="2">
-        <v>116756</v>
-      </c>
-      <c r="H8" s="3">
-        <v>44881.24546290509</v>
-      </c>
-      <c r="I8" s="3">
-        <v>44881.2454641088</v>
+        <v>44881.521820486116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted price in orderItem
</commit_message>
<xml_diff>
--- a/server/files/orders.xlsx
+++ b/server/files/orders.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>No</t>
   </si>
@@ -40,25 +40,31 @@
     <t>O'zgartirilgan sana</t>
   </si>
   <si>
-    <t>Mashrab</t>
-  </si>
-  <si>
-    <t>+998946775454</t>
-  </si>
-  <si>
-    <t>STORE_OWNER: sinadigan narsa bor COURIER: Sotildi</t>
-  </si>
-  <si>
-    <t>SOLD</t>
-  </si>
-  <si>
-    <t>Baxrom</t>
-  </si>
-  <si>
-    <t>+998936979876</t>
-  </si>
-  <si>
-    <t>STORE_OWNER: klient1 COURIER: Sotildi</t>
+    <t>vcxvcvcxv</t>
+  </si>
+  <si>
+    <t>+998939950036</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: fdsfdsf</t>
+  </si>
+  <si>
+    <t>ACCEPTED</t>
+  </si>
+  <si>
+    <t>recipient</t>
+  </si>
+  <si>
+    <t>+998939950202</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: undefined</t>
+  </si>
+  <si>
+    <t>ssss</t>
+  </si>
+  <si>
+    <t>STORE_OWNER: 232</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -502,16 +508,16 @@
         <v>12</v>
       </c>
       <c r="F2" s="2">
-        <v>70000</v>
+        <v>50000</v>
       </c>
       <c r="G2" s="2">
-        <v>19536</v>
+        <v>3434</v>
       </c>
       <c r="H2" s="3">
-        <v>44881.27319835648</v>
+        <v>44882.50939576389</v>
       </c>
       <c r="I2" s="3">
-        <v>44881.46914159722</v>
+        <v>44882.51629447917</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -534,13 +540,13 @@
         <v>50000</v>
       </c>
       <c r="G3" s="2">
-        <v>10656</v>
+        <v>557577</v>
       </c>
       <c r="H3" s="3">
-        <v>44881.271496030095</v>
+        <v>44882.511876793986</v>
       </c>
       <c r="I3" s="3">
-        <v>44881.279108414354</v>
+        <v>44882.51630575232</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -563,13 +569,100 @@
         <v>50000</v>
       </c>
       <c r="G4" s="2">
-        <v>773256</v>
+        <v>557577</v>
       </c>
       <c r="H4" s="3">
-        <v>44881.3988674537</v>
+        <v>44882.511935208335</v>
       </c>
       <c r="I4" s="3">
-        <v>44881.46670815972</v>
+        <v>44882.51632061343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2">
+        <v>50000</v>
+      </c>
+      <c r="G5" s="2">
+        <v>557577</v>
+      </c>
+      <c r="H5" s="3">
+        <v>44882.51194377315</v>
+      </c>
+      <c r="I5" s="3">
+        <v>44882.51632913195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <v>50000</v>
+      </c>
+      <c r="G6" s="2">
+        <v>557577</v>
+      </c>
+      <c r="H6" s="3">
+        <v>44882.51195315972</v>
+      </c>
+      <c r="I6" s="3">
+        <v>44882.51633701389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2">
+        <v>50000</v>
+      </c>
+      <c r="G7" s="2">
+        <v>433443</v>
+      </c>
+      <c r="H7" s="3">
+        <v>44882.51458509259</v>
+      </c>
+      <c r="I7" s="3">
+        <v>44882.51634814814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>